<commit_message>
updating APP_CDD and adding APP_TEST(version 1)
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/RTM_2.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/RTM_2.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="2565"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -105,9 +106,6 @@
     <t>project manager</t>
   </si>
   <si>
-    <t>Sef eldin ahmed</t>
-  </si>
-  <si>
     <t xml:space="preserve">void TIMER_ISR(void)
 </t>
   </si>
@@ -194,6 +192,9 @@
   </si>
   <si>
     <t>APP_voidInit()</t>
+  </si>
+  <si>
+    <t>Sef eldin Ahmed</t>
   </si>
 </sst>
 </file>
@@ -469,6 +470,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -486,15 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -802,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +840,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="G3" s="24"/>
     </row>
@@ -857,7 +858,7 @@
         <v>18</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>19</v>
@@ -902,17 +903,17 @@
       <c r="AK5" s="9"/>
     </row>
     <row r="6" spans="1:37" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="30" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>36</v>
+      <c r="C6" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>35</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="6"/>
@@ -951,15 +952,15 @@
       <c r="AK6" s="1"/>
     </row>
     <row r="7" spans="1:37" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="31"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>37</v>
+      <c r="C7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -998,15 +999,15 @@
       <c r="AK7" s="1"/>
     </row>
     <row r="8" spans="1:37" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>38</v>
+      <c r="C8" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
@@ -1045,17 +1046,17 @@
       <c r="AK8" s="1"/>
     </row>
     <row r="9" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="33" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="33" t="s">
         <v>39</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>38</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
@@ -1094,15 +1095,15 @@
       <c r="AK9" s="1"/>
     </row>
     <row r="10" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
+      <c r="A10" s="34"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="33" t="s">
         <v>41</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="3"/>
@@ -1141,15 +1142,15 @@
       <c r="AK10" s="1"/>
     </row>
     <row r="11" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
+      <c r="A11" s="34"/>
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>42</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
@@ -1188,15 +1189,15 @@
       <c r="AK11" s="1"/>
     </row>
     <row r="12" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+      <c r="A12" s="34"/>
       <c r="B12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="33" t="s">
         <v>44</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
@@ -1235,15 +1236,15 @@
       <c r="AK12" s="1"/>
     </row>
     <row r="13" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="33" t="s">
         <v>46</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
@@ -1282,15 +1283,15 @@
       <c r="AK13" s="1"/>
     </row>
     <row r="14" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
+      <c r="A14" s="35"/>
       <c r="B14" s="12" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="33" t="s">
-        <v>48</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
@@ -1329,17 +1330,17 @@
       <c r="AK14" s="1"/>
     </row>
     <row r="15" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>49</v>
-      </c>
-      <c r="D15" s="33" t="s">
-        <v>50</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
@@ -1378,15 +1379,15 @@
       <c r="AK15" s="1"/>
     </row>
     <row r="16" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="33" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
@@ -1425,15 +1426,15 @@
       <c r="AK16" s="1"/>
     </row>
     <row r="17" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="34"/>
       <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="27" t="s">
         <v>52</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>53</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="3"/>
@@ -1472,15 +1473,15 @@
       <c r="AK17" s="1"/>
     </row>
     <row r="18" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="27" t="s">
         <v>54</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>55</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="13"/>
@@ -1526,10 +1527,10 @@
         <v>14</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" s="33" t="s">
         <v>56</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>55</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="26"/>

</xml_diff>

<commit_message>
RTM updated with the test cases states
</commit_message>
<xml_diff>
--- a/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/RTM_2.xlsx
+++ b/SOFTWARE_ENGINEERING_PROJECT/PROJECT_DOCUMENTATION/RTM_2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="2565"/>
@@ -11,13 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>CR_001</t>
   </si>
@@ -64,9 +63,6 @@
     <t>SR4_A01</t>
   </si>
   <si>
-    <t>Test Cases</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -76,9 +72,6 @@
     <t>API's</t>
   </si>
   <si>
-    <t>Design pattern</t>
-  </si>
-  <si>
     <t>SR3_A04</t>
   </si>
   <si>
@@ -106,28 +99,13 @@
     <t>project manager</t>
   </si>
   <si>
-    <t xml:space="preserve">void TIMER_ISR(void)
-</t>
-  </si>
-  <si>
     <t>APP_u32Convertto24hourssystem()</t>
   </si>
   <si>
-    <t xml:space="preserve">extern void APP_u8TimeUpdate();
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extern void APP_voidDisplay();
-</t>
-  </si>
-  <si>
     <t>APP_voidDisplay()</t>
   </si>
   <si>
     <t>line of code (filename/lineNo.)</t>
-  </si>
-  <si>
-    <t>APP_Functions.c/ "30"</t>
   </si>
   <si>
     <t>APP_Functions.c/ "76"</t>
@@ -195,13 +173,61 @@
   </si>
   <si>
     <t>Sef eldin Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APP_voidUpdateTimers()
+</t>
+  </si>
+  <si>
+    <t>APP_Functions.c/ "168"</t>
+  </si>
+  <si>
+    <t>TC_APP_08</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> APP_u8TimeUpdate();
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> APP_voidDisplay();
+</t>
+  </si>
+  <si>
+    <t>TC_APP_12</t>
+  </si>
+  <si>
+    <t>TC_APP_09</t>
+  </si>
+  <si>
+    <t>TC_APP_10</t>
+  </si>
+  <si>
+    <t>TC_APP_06</t>
+  </si>
+  <si>
+    <t>TC_APP_11</t>
+  </si>
+  <si>
+    <t>TC_APP_14</t>
+  </si>
+  <si>
+    <t>TC_APP_07</t>
+  </si>
+  <si>
+    <t>TC_APP_01</t>
+  </si>
+  <si>
+    <t>Test cases ID</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +258,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,8 +310,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -391,24 +431,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -416,27 +443,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -459,17 +480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -496,6 +506,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -800,127 +834,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK331"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AJ331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="36.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="74.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="52.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="22" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="52.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="34" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="G1" s="24"/>
-    </row>
-    <row r="2" spans="1:37" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+    <row r="1" spans="1:36" ht="27" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B1" s="15"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="2" spans="1:36" ht="22.5" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="31"/>
+    </row>
+    <row r="3" spans="1:36" ht="18.75" customHeight="1">
+      <c r="A3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:37" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="G3" s="24"/>
-    </row>
-    <row r="4" spans="1:37" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="24"/>
-    </row>
-    <row r="5" spans="1:37" s="10" customFormat="1" ht="49.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="11" t="s">
+      <c r="B3" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="31"/>
+    </row>
+    <row r="4" spans="1:36" ht="33.75" customHeight="1">
+      <c r="F4" s="31"/>
+    </row>
+    <row r="5" spans="1:36" s="8" customFormat="1" ht="49.15" customHeight="1">
+      <c r="A5" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="C5" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
-      <c r="W5" s="9"/>
-      <c r="X5" s="9"/>
-      <c r="Y5" s="9"/>
-      <c r="Z5" s="9"/>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9"/>
-      <c r="AC5" s="9"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
-      <c r="AF5" s="9"/>
-      <c r="AG5" s="9"/>
-      <c r="AH5" s="9"/>
-      <c r="AI5" s="9"/>
-      <c r="AJ5" s="9"/>
-      <c r="AK5" s="9"/>
-    </row>
-    <row r="6" spans="1:37" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="7"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+    </row>
+    <row r="6" spans="1:36" ht="36.75" customHeight="1">
+      <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="23">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7"/>
+      <c r="C6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -949,25 +983,28 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
       <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-    </row>
-    <row r="7" spans="1:37" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+    </row>
+    <row r="7" spans="1:36" ht="42.75" customHeight="1">
+      <c r="A7" s="22"/>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="23">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8"/>
+      <c r="C7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -996,25 +1033,28 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-    </row>
-    <row r="8" spans="1:37" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="12" t="s">
+    </row>
+    <row r="8" spans="1:36" ht="29.25" customHeight="1">
+      <c r="A8" s="23"/>
+      <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="23">
-        <v>0</v>
-      </c>
-      <c r="H8" s="14"/>
+      <c r="C8" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="32">
+        <v>1</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1043,27 +1083,30 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-    </row>
-    <row r="9" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+    </row>
+    <row r="9" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A9" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="23">
-        <v>0</v>
-      </c>
-      <c r="H9" s="7"/>
+      <c r="C9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="32">
+        <v>1</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1092,25 +1135,28 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-    </row>
-    <row r="10" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+    </row>
+    <row r="10" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A10" s="25"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="23">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8"/>
+      <c r="C10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1139,25 +1185,28 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-    </row>
-    <row r="11" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="4" t="s">
+    </row>
+    <row r="11" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A11" s="25"/>
+      <c r="B11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="23">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8"/>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="32">
+        <v>1</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -1186,25 +1235,28 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
       <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-    </row>
-    <row r="12" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34"/>
-      <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="23">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8"/>
+    </row>
+    <row r="12" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A12" s="25"/>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1233,25 +1285,28 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
       <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-    </row>
-    <row r="13" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34"/>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="23">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8"/>
+    </row>
+    <row r="13" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A13" s="25"/>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="32">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1280,25 +1335,28 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
       <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
-    </row>
-    <row r="14" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="35"/>
-      <c r="B14" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="23">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14"/>
+    </row>
+    <row r="14" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A14" s="26"/>
+      <c r="B14" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="32">
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1327,27 +1385,30 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
       <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
-    </row>
-    <row r="15" spans="1:37" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+    </row>
+    <row r="15" spans="1:36" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="23">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7"/>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1376,25 +1437,28 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
       <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
-    </row>
-    <row r="16" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
-      <c r="B16" s="4" t="s">
+    </row>
+    <row r="16" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A16" s="25"/>
+      <c r="B16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="23">
-        <v>0</v>
-      </c>
-      <c r="H16" s="8"/>
+      <c r="C16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="32">
+        <v>0.33</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1423,25 +1487,28 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
-      <c r="AK16" s="1"/>
-    </row>
-    <row r="17" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34"/>
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="17" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A17" s="25"/>
+      <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="4"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="23">
-        <v>0</v>
-      </c>
-      <c r="H17" s="8"/>
+      <c r="C17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0.67</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1470,25 +1537,28 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
       <c r="AJ17" s="1"/>
-      <c r="AK17" s="1"/>
-    </row>
-    <row r="18" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="23">
-        <v>0</v>
-      </c>
-      <c r="H18" s="14"/>
+    </row>
+    <row r="18" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A18" s="26"/>
+      <c r="B18" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="32">
+        <v>1</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1517,27 +1587,30 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
       <c r="AJ18" s="1"/>
-      <c r="AK18" s="1"/>
-    </row>
-    <row r="19" spans="1:37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    </row>
+    <row r="19" spans="1:36" ht="24.95" customHeight="1">
+      <c r="A19" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="23">
-        <v>0</v>
-      </c>
-      <c r="H19" s="25"/>
+      <c r="C19" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="33">
+        <v>1</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1566,10 +1639,10 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
       <c r="AJ19" s="1"/>
-      <c r="AK19" s="1"/>
-    </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G20" s="24"/>
+    </row>
+    <row r="20" spans="1:36">
+      <c r="F20" s="31"/>
+      <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1598,10 +1671,10 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
       <c r="AJ20" s="1"/>
-      <c r="AK20" s="1"/>
-    </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G21" s="24"/>
+    </row>
+    <row r="21" spans="1:36">
+      <c r="F21" s="31"/>
+      <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1630,10 +1703,10 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
       <c r="AJ21" s="1"/>
-      <c r="AK21" s="1"/>
-    </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G22" s="24"/>
+    </row>
+    <row r="22" spans="1:36">
+      <c r="F22" s="31"/>
+      <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1662,10 +1735,10 @@
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
       <c r="AJ22" s="1"/>
-      <c r="AK22" s="1"/>
-    </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G23" s="24"/>
+    </row>
+    <row r="23" spans="1:36">
+      <c r="F23" s="31"/>
+      <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1694,10 +1767,10 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
       <c r="AJ23" s="1"/>
-      <c r="AK23" s="1"/>
-    </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G24" s="24"/>
+    </row>
+    <row r="24" spans="1:36">
+      <c r="F24" s="31"/>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1726,10 +1799,10 @@
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
       <c r="AJ24" s="1"/>
-      <c r="AK24" s="1"/>
-    </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G25" s="24"/>
+    </row>
+    <row r="25" spans="1:36">
+      <c r="F25" s="31"/>
+      <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1758,10 +1831,10 @@
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
       <c r="AJ25" s="1"/>
-      <c r="AK25" s="1"/>
-    </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G26" s="24"/>
+    </row>
+    <row r="26" spans="1:36">
+      <c r="F26" s="31"/>
+      <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1790,10 +1863,10 @@
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
       <c r="AJ26" s="1"/>
-      <c r="AK26" s="1"/>
-    </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G27" s="24"/>
+    </row>
+    <row r="27" spans="1:36">
+      <c r="F27" s="31"/>
+      <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1822,10 +1895,10 @@
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
       <c r="AJ27" s="1"/>
-      <c r="AK27" s="1"/>
-    </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G28" s="24"/>
+    </row>
+    <row r="28" spans="1:36">
+      <c r="F28" s="31"/>
+      <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1854,10 +1927,10 @@
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
       <c r="AJ28" s="1"/>
-      <c r="AK28" s="1"/>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G29" s="24"/>
+    </row>
+    <row r="29" spans="1:36">
+      <c r="F29" s="31"/>
+      <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -1886,10 +1959,10 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
       <c r="AJ29" s="1"/>
-      <c r="AK29" s="1"/>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G30" s="24"/>
+    </row>
+    <row r="30" spans="1:36">
+      <c r="F30" s="31"/>
+      <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -1918,10 +1991,10 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
       <c r="AJ30" s="1"/>
-      <c r="AK30" s="1"/>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G31" s="24"/>
+    </row>
+    <row r="31" spans="1:36">
+      <c r="F31" s="31"/>
+      <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1950,10 +2023,10 @@
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
       <c r="AJ31" s="1"/>
-      <c r="AK31" s="1"/>
-    </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="G32" s="24"/>
+    </row>
+    <row r="32" spans="1:36">
+      <c r="F32" s="31"/>
+      <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -1982,10 +2055,10 @@
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
       <c r="AJ32" s="1"/>
-      <c r="AK32" s="1"/>
-    </row>
-    <row r="33" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G33" s="24"/>
+    </row>
+    <row r="33" spans="6:36">
+      <c r="F33" s="31"/>
+      <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2014,10 +2087,10 @@
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
       <c r="AJ33" s="1"/>
-      <c r="AK33" s="1"/>
-    </row>
-    <row r="34" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G34" s="24"/>
+    </row>
+    <row r="34" spans="6:36">
+      <c r="F34" s="31"/>
+      <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -2046,10 +2119,10 @@
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
       <c r="AJ34" s="1"/>
-      <c r="AK34" s="1"/>
-    </row>
-    <row r="35" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G35" s="24"/>
+    </row>
+    <row r="35" spans="6:36">
+      <c r="F35" s="31"/>
+      <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2078,10 +2151,10 @@
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
       <c r="AJ35" s="1"/>
-      <c r="AK35" s="1"/>
-    </row>
-    <row r="36" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G36" s="24"/>
+    </row>
+    <row r="36" spans="6:36">
+      <c r="F36" s="31"/>
+      <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2110,10 +2183,10 @@
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
       <c r="AJ36" s="1"/>
-      <c r="AK36" s="1"/>
-    </row>
-    <row r="37" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G37" s="24"/>
+    </row>
+    <row r="37" spans="6:36">
+      <c r="F37" s="31"/>
+      <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2142,10 +2215,10 @@
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
       <c r="AJ37" s="1"/>
-      <c r="AK37" s="1"/>
-    </row>
-    <row r="38" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G38" s="24"/>
+    </row>
+    <row r="38" spans="6:36">
+      <c r="F38" s="31"/>
+      <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2174,10 +2247,10 @@
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
-      <c r="AK38" s="1"/>
-    </row>
-    <row r="39" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G39" s="24"/>
+    </row>
+    <row r="39" spans="6:36">
+      <c r="F39" s="31"/>
+      <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2206,10 +2279,10 @@
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
       <c r="AJ39" s="1"/>
-      <c r="AK39" s="1"/>
-    </row>
-    <row r="40" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G40" s="24"/>
+    </row>
+    <row r="40" spans="6:36">
+      <c r="F40" s="31"/>
+      <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2238,10 +2311,10 @@
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
       <c r="AJ40" s="1"/>
-      <c r="AK40" s="1"/>
-    </row>
-    <row r="41" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G41" s="24"/>
+    </row>
+    <row r="41" spans="6:36">
+      <c r="F41" s="31"/>
+      <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2270,10 +2343,10 @@
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
       <c r="AJ41" s="1"/>
-      <c r="AK41" s="1"/>
-    </row>
-    <row r="42" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G42" s="24"/>
+    </row>
+    <row r="42" spans="6:36">
+      <c r="F42" s="31"/>
+      <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2302,10 +2375,10 @@
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
       <c r="AJ42" s="1"/>
-      <c r="AK42" s="1"/>
-    </row>
-    <row r="43" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G43" s="24"/>
+    </row>
+    <row r="43" spans="6:36">
+      <c r="F43" s="31"/>
+      <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -2334,10 +2407,10 @@
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
       <c r="AJ43" s="1"/>
-      <c r="AK43" s="1"/>
-    </row>
-    <row r="44" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G44" s="24"/>
+    </row>
+    <row r="44" spans="6:36">
+      <c r="F44" s="31"/>
+      <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -2366,10 +2439,10 @@
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
       <c r="AJ44" s="1"/>
-      <c r="AK44" s="1"/>
-    </row>
-    <row r="45" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G45" s="24"/>
+    </row>
+    <row r="45" spans="6:36">
+      <c r="F45" s="31"/>
+      <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -2398,10 +2471,10 @@
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
       <c r="AJ45" s="1"/>
-      <c r="AK45" s="1"/>
-    </row>
-    <row r="46" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G46" s="24"/>
+    </row>
+    <row r="46" spans="6:36">
+      <c r="F46" s="31"/>
+      <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -2430,10 +2503,10 @@
       <c r="AH46" s="1"/>
       <c r="AI46" s="1"/>
       <c r="AJ46" s="1"/>
-      <c r="AK46" s="1"/>
-    </row>
-    <row r="47" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G47" s="24"/>
+    </row>
+    <row r="47" spans="6:36">
+      <c r="F47" s="31"/>
+      <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -2462,10 +2535,10 @@
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
       <c r="AJ47" s="1"/>
-      <c r="AK47" s="1"/>
-    </row>
-    <row r="48" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G48" s="24"/>
+    </row>
+    <row r="48" spans="6:36">
+      <c r="F48" s="31"/>
+      <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -2494,10 +2567,10 @@
       <c r="AH48" s="1"/>
       <c r="AI48" s="1"/>
       <c r="AJ48" s="1"/>
-      <c r="AK48" s="1"/>
-    </row>
-    <row r="49" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G49" s="24"/>
+    </row>
+    <row r="49" spans="6:36">
+      <c r="F49" s="31"/>
+      <c r="H49" s="1"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -2526,10 +2599,10 @@
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
       <c r="AJ49" s="1"/>
-      <c r="AK49" s="1"/>
-    </row>
-    <row r="50" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G50" s="24"/>
+    </row>
+    <row r="50" spans="6:36">
+      <c r="F50" s="31"/>
+      <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -2558,10 +2631,10 @@
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
       <c r="AJ50" s="1"/>
-      <c r="AK50" s="1"/>
-    </row>
-    <row r="51" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G51" s="24"/>
+    </row>
+    <row r="51" spans="6:36">
+      <c r="F51" s="31"/>
+      <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -2590,10 +2663,10 @@
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
       <c r="AJ51" s="1"/>
-      <c r="AK51" s="1"/>
-    </row>
-    <row r="52" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G52" s="24"/>
+    </row>
+    <row r="52" spans="6:36">
+      <c r="F52" s="31"/>
+      <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -2622,10 +2695,10 @@
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
       <c r="AJ52" s="1"/>
-      <c r="AK52" s="1"/>
-    </row>
-    <row r="53" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G53" s="24"/>
+    </row>
+    <row r="53" spans="6:36">
+      <c r="F53" s="31"/>
+      <c r="H53" s="1"/>
       <c r="I53" s="1"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -2654,841 +2727,840 @@
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
       <c r="AJ53" s="1"/>
-      <c r="AK53" s="1"/>
-    </row>
-    <row r="54" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G54" s="24"/>
-    </row>
-    <row r="55" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G55" s="24"/>
-    </row>
-    <row r="56" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G56" s="24"/>
-    </row>
-    <row r="57" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G57" s="24"/>
-    </row>
-    <row r="58" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G58" s="24"/>
-    </row>
-    <row r="59" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G59" s="24"/>
-    </row>
-    <row r="60" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G60" s="24"/>
-    </row>
-    <row r="61" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G61" s="24"/>
-    </row>
-    <row r="62" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G62" s="24"/>
-    </row>
-    <row r="63" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G63" s="24"/>
-    </row>
-    <row r="64" spans="7:37" x14ac:dyDescent="0.25">
-      <c r="G64" s="24"/>
-    </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G65" s="24"/>
-    </row>
-    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G66" s="24"/>
-    </row>
-    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G67" s="24"/>
-    </row>
-    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G68" s="24"/>
-    </row>
-    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G69" s="24"/>
-    </row>
-    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G70" s="24"/>
-    </row>
-    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G71" s="24"/>
-    </row>
-    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G72" s="24"/>
-    </row>
-    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G73" s="24"/>
-    </row>
-    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G74" s="24"/>
-    </row>
-    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G75" s="24"/>
-    </row>
-    <row r="76" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G76" s="24"/>
-    </row>
-    <row r="77" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G77" s="24"/>
-    </row>
-    <row r="78" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G78" s="24"/>
-    </row>
-    <row r="79" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G79" s="24"/>
-    </row>
-    <row r="80" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G80" s="24"/>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G81" s="24"/>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G82" s="24"/>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G83" s="24"/>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G84" s="24"/>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G85" s="24"/>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G86" s="24"/>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G87" s="24"/>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G88" s="24"/>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G89" s="24"/>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G90" s="24"/>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G91" s="24"/>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G92" s="24"/>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G93" s="24"/>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G94" s="24"/>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G95" s="24"/>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G96" s="24"/>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G97" s="24"/>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G98" s="24"/>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G99" s="24"/>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G100" s="24"/>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G101" s="24"/>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G102" s="24"/>
-    </row>
-    <row r="103" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G103" s="24"/>
-    </row>
-    <row r="104" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G104" s="24"/>
-    </row>
-    <row r="105" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G105" s="24"/>
-    </row>
-    <row r="106" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G106" s="24"/>
-    </row>
-    <row r="107" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G107" s="24"/>
-    </row>
-    <row r="108" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G108" s="24"/>
-    </row>
-    <row r="109" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G109" s="24"/>
-    </row>
-    <row r="110" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G110" s="24"/>
-    </row>
-    <row r="111" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G111" s="24"/>
-    </row>
-    <row r="112" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G112" s="24"/>
-    </row>
-    <row r="113" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G113" s="24"/>
-    </row>
-    <row r="114" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G114" s="24"/>
-    </row>
-    <row r="115" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G115" s="24"/>
-    </row>
-    <row r="116" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G116" s="24"/>
-    </row>
-    <row r="117" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G117" s="24"/>
-    </row>
-    <row r="118" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G118" s="24"/>
-    </row>
-    <row r="119" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G119" s="24"/>
-    </row>
-    <row r="120" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G120" s="24"/>
-    </row>
-    <row r="121" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G121" s="24"/>
-    </row>
-    <row r="122" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G122" s="24"/>
-    </row>
-    <row r="123" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G123" s="24"/>
-    </row>
-    <row r="124" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G124" s="24"/>
-    </row>
-    <row r="125" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G125" s="24"/>
-    </row>
-    <row r="126" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G126" s="24"/>
-    </row>
-    <row r="127" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G127" s="24"/>
-    </row>
-    <row r="128" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G128" s="24"/>
-    </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G129" s="24"/>
-    </row>
-    <row r="130" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G130" s="24"/>
-    </row>
-    <row r="131" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G131" s="24"/>
-    </row>
-    <row r="132" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G132" s="24"/>
-    </row>
-    <row r="133" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G133" s="24"/>
-    </row>
-    <row r="134" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G134" s="24"/>
-    </row>
-    <row r="135" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G135" s="24"/>
-    </row>
-    <row r="136" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G136" s="24"/>
-    </row>
-    <row r="137" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G137" s="24"/>
-    </row>
-    <row r="138" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G138" s="24"/>
-    </row>
-    <row r="139" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G139" s="24"/>
-    </row>
-    <row r="140" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G140" s="24"/>
-    </row>
-    <row r="141" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G141" s="24"/>
-    </row>
-    <row r="142" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G142" s="24"/>
-    </row>
-    <row r="143" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G143" s="24"/>
-    </row>
-    <row r="144" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G144" s="24"/>
-    </row>
-    <row r="145" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G145" s="24"/>
-    </row>
-    <row r="146" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G146" s="24"/>
-    </row>
-    <row r="147" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G147" s="24"/>
-    </row>
-    <row r="148" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G148" s="24"/>
-    </row>
-    <row r="149" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G149" s="24"/>
-    </row>
-    <row r="150" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G150" s="24"/>
-    </row>
-    <row r="151" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G151" s="24"/>
-    </row>
-    <row r="152" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G152" s="24"/>
-    </row>
-    <row r="153" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G153" s="24"/>
-    </row>
-    <row r="154" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G154" s="24"/>
-    </row>
-    <row r="155" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G155" s="24"/>
-    </row>
-    <row r="156" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G156" s="24"/>
-    </row>
-    <row r="157" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G157" s="24"/>
-    </row>
-    <row r="158" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G158" s="24"/>
-    </row>
-    <row r="159" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G159" s="24"/>
-    </row>
-    <row r="160" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G160" s="24"/>
-    </row>
-    <row r="161" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G161" s="24"/>
-    </row>
-    <row r="162" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G162" s="24"/>
-    </row>
-    <row r="163" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G163" s="24"/>
-    </row>
-    <row r="164" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G164" s="24"/>
-    </row>
-    <row r="165" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G165" s="24"/>
-    </row>
-    <row r="166" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G166" s="24"/>
-    </row>
-    <row r="167" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G167" s="24"/>
-    </row>
-    <row r="168" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G168" s="24"/>
-    </row>
-    <row r="169" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G169" s="24"/>
-    </row>
-    <row r="170" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G170" s="24"/>
-    </row>
-    <row r="171" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G171" s="24"/>
-    </row>
-    <row r="172" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G172" s="24"/>
-    </row>
-    <row r="173" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G173" s="24"/>
-    </row>
-    <row r="174" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G174" s="24"/>
-    </row>
-    <row r="175" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G175" s="24"/>
-    </row>
-    <row r="176" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G176" s="24"/>
-    </row>
-    <row r="177" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G177" s="24"/>
-    </row>
-    <row r="178" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G178" s="24"/>
-    </row>
-    <row r="179" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G179" s="24"/>
-    </row>
-    <row r="180" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G180" s="24"/>
-    </row>
-    <row r="181" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G181" s="24"/>
-    </row>
-    <row r="182" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G182" s="24"/>
-    </row>
-    <row r="183" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G183" s="24"/>
-    </row>
-    <row r="184" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G184" s="24"/>
-    </row>
-    <row r="185" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G185" s="24"/>
-    </row>
-    <row r="186" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G186" s="24"/>
-    </row>
-    <row r="187" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G187" s="24"/>
-    </row>
-    <row r="188" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G188" s="24"/>
-    </row>
-    <row r="189" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G189" s="24"/>
-    </row>
-    <row r="190" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G190" s="24"/>
-    </row>
-    <row r="191" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G191" s="24"/>
-    </row>
-    <row r="192" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G192" s="24"/>
-    </row>
-    <row r="193" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G193" s="24"/>
-    </row>
-    <row r="194" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G194" s="24"/>
-    </row>
-    <row r="195" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G195" s="24"/>
-    </row>
-    <row r="196" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G196" s="24"/>
-    </row>
-    <row r="197" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G197" s="24"/>
-    </row>
-    <row r="198" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G198" s="24"/>
-    </row>
-    <row r="199" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G199" s="24"/>
-    </row>
-    <row r="200" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G200" s="24"/>
-    </row>
-    <row r="201" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G201" s="24"/>
-    </row>
-    <row r="202" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G202" s="24"/>
-    </row>
-    <row r="203" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G203" s="24"/>
-    </row>
-    <row r="204" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G204" s="24"/>
-    </row>
-    <row r="205" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G205" s="24"/>
-    </row>
-    <row r="206" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G206" s="24"/>
-    </row>
-    <row r="207" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G207" s="24"/>
-    </row>
-    <row r="208" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G208" s="24"/>
-    </row>
-    <row r="209" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G209" s="24"/>
-    </row>
-    <row r="210" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G210" s="24"/>
-    </row>
-    <row r="211" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G211" s="24"/>
-    </row>
-    <row r="212" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G212" s="24"/>
-    </row>
-    <row r="213" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G213" s="24"/>
-    </row>
-    <row r="214" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G214" s="24"/>
-    </row>
-    <row r="215" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G215" s="24"/>
-    </row>
-    <row r="216" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G216" s="24"/>
-    </row>
-    <row r="217" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G217" s="24"/>
-    </row>
-    <row r="218" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G218" s="24"/>
-    </row>
-    <row r="219" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G219" s="24"/>
-    </row>
-    <row r="220" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G220" s="24"/>
-    </row>
-    <row r="221" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G221" s="24"/>
-    </row>
-    <row r="222" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G222" s="24"/>
-    </row>
-    <row r="223" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G223" s="24"/>
-    </row>
-    <row r="224" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G224" s="24"/>
-    </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G225" s="24"/>
-    </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G226" s="24"/>
-    </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G227" s="24"/>
-    </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G228" s="24"/>
-    </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G229" s="24"/>
-    </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G230" s="24"/>
-    </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G231" s="24"/>
-    </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G232" s="24"/>
-    </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G233" s="24"/>
-    </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G234" s="24"/>
-    </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G235" s="24"/>
-    </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G236" s="24"/>
-    </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G237" s="24"/>
-    </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G238" s="24"/>
-    </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G239" s="24"/>
-    </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G240" s="24"/>
-    </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G241" s="24"/>
-    </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G242" s="24"/>
-    </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G243" s="24"/>
-    </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G244" s="24"/>
-    </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G245" s="24"/>
-    </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G246" s="24"/>
-    </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G247" s="24"/>
-    </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G248" s="24"/>
-    </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G249" s="24"/>
-    </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G250" s="24"/>
-    </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G251" s="24"/>
-    </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G252" s="24"/>
-    </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G253" s="24"/>
-    </row>
-    <row r="254" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G254" s="24"/>
-    </row>
-    <row r="255" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G255" s="24"/>
-    </row>
-    <row r="256" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G256" s="24"/>
-    </row>
-    <row r="257" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G257" s="24"/>
-    </row>
-    <row r="258" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G258" s="24"/>
-    </row>
-    <row r="259" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G259" s="24"/>
-    </row>
-    <row r="260" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G260" s="24"/>
-    </row>
-    <row r="261" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G261" s="24"/>
-    </row>
-    <row r="262" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G262" s="24"/>
-    </row>
-    <row r="263" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G263" s="24"/>
-    </row>
-    <row r="264" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G264" s="24"/>
-    </row>
-    <row r="265" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G265" s="24"/>
-    </row>
-    <row r="266" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G266" s="24"/>
-    </row>
-    <row r="267" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G267" s="24"/>
-    </row>
-    <row r="268" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G268" s="24"/>
-    </row>
-    <row r="269" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G269" s="24"/>
-    </row>
-    <row r="270" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G270" s="24"/>
-    </row>
-    <row r="271" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G271" s="24"/>
-    </row>
-    <row r="272" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G272" s="24"/>
-    </row>
-    <row r="273" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G273" s="24"/>
-    </row>
-    <row r="274" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G274" s="24"/>
-    </row>
-    <row r="275" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G275" s="24"/>
-    </row>
-    <row r="276" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G276" s="24"/>
-    </row>
-    <row r="277" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G277" s="24"/>
-    </row>
-    <row r="278" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G278" s="24"/>
-    </row>
-    <row r="279" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G279" s="24"/>
-    </row>
-    <row r="280" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G280" s="24"/>
-    </row>
-    <row r="281" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G281" s="24"/>
-    </row>
-    <row r="282" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G282" s="24"/>
-    </row>
-    <row r="283" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G283" s="24"/>
-    </row>
-    <row r="284" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G284" s="24"/>
-    </row>
-    <row r="285" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G285" s="24"/>
-    </row>
-    <row r="286" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G286" s="24"/>
-    </row>
-    <row r="287" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G287" s="24"/>
-    </row>
-    <row r="288" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G288" s="24"/>
-    </row>
-    <row r="289" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G289" s="24"/>
-    </row>
-    <row r="290" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G290" s="24"/>
-    </row>
-    <row r="291" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G291" s="24"/>
-    </row>
-    <row r="292" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G292" s="24"/>
-    </row>
-    <row r="293" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G293" s="24"/>
-    </row>
-    <row r="294" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G294" s="24"/>
-    </row>
-    <row r="295" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G295" s="24"/>
-    </row>
-    <row r="296" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G296" s="24"/>
-    </row>
-    <row r="297" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G297" s="24"/>
-    </row>
-    <row r="298" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G298" s="24"/>
-    </row>
-    <row r="299" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G299" s="24"/>
-    </row>
-    <row r="300" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G300" s="24"/>
-    </row>
-    <row r="301" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G301" s="24"/>
-    </row>
-    <row r="302" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G302" s="24"/>
-    </row>
-    <row r="303" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G303" s="24"/>
-    </row>
-    <row r="304" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G304" s="24"/>
-    </row>
-    <row r="305" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G305" s="24"/>
-    </row>
-    <row r="306" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G306" s="24"/>
-    </row>
-    <row r="307" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G307" s="24"/>
-    </row>
-    <row r="308" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G308" s="24"/>
-    </row>
-    <row r="309" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G309" s="24"/>
-    </row>
-    <row r="310" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G310" s="24"/>
-    </row>
-    <row r="311" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G311" s="24"/>
-    </row>
-    <row r="312" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G312" s="24"/>
-    </row>
-    <row r="313" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G313" s="24"/>
-    </row>
-    <row r="314" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G314" s="24"/>
-    </row>
-    <row r="315" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G315" s="24"/>
-    </row>
-    <row r="316" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G316" s="24"/>
-    </row>
-    <row r="317" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G317" s="24"/>
-    </row>
-    <row r="318" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G318" s="24"/>
-    </row>
-    <row r="319" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G319" s="24"/>
-    </row>
-    <row r="320" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G320" s="24"/>
-    </row>
-    <row r="321" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G321" s="24"/>
-    </row>
-    <row r="322" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G322" s="24"/>
-    </row>
-    <row r="323" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G323" s="24"/>
-    </row>
-    <row r="324" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G324" s="24"/>
-    </row>
-    <row r="325" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G325" s="24"/>
-    </row>
-    <row r="326" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G326" s="24"/>
-    </row>
-    <row r="327" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G327" s="24"/>
-    </row>
-    <row r="328" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G328" s="24"/>
-    </row>
-    <row r="329" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G329" s="24"/>
-    </row>
-    <row r="330" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G330" s="24"/>
-    </row>
-    <row r="331" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G331" s="24"/>
+    </row>
+    <row r="54" spans="6:36">
+      <c r="F54" s="31"/>
+    </row>
+    <row r="55" spans="6:36">
+      <c r="F55" s="31"/>
+    </row>
+    <row r="56" spans="6:36">
+      <c r="F56" s="31"/>
+    </row>
+    <row r="57" spans="6:36">
+      <c r="F57" s="31"/>
+    </row>
+    <row r="58" spans="6:36">
+      <c r="F58" s="31"/>
+    </row>
+    <row r="59" spans="6:36">
+      <c r="F59" s="31"/>
+    </row>
+    <row r="60" spans="6:36">
+      <c r="F60" s="31"/>
+    </row>
+    <row r="61" spans="6:36">
+      <c r="F61" s="31"/>
+    </row>
+    <row r="62" spans="6:36">
+      <c r="F62" s="31"/>
+    </row>
+    <row r="63" spans="6:36">
+      <c r="F63" s="31"/>
+    </row>
+    <row r="64" spans="6:36">
+      <c r="F64" s="31"/>
+    </row>
+    <row r="65" spans="6:6">
+      <c r="F65" s="31"/>
+    </row>
+    <row r="66" spans="6:6">
+      <c r="F66" s="31"/>
+    </row>
+    <row r="67" spans="6:6">
+      <c r="F67" s="31"/>
+    </row>
+    <row r="68" spans="6:6">
+      <c r="F68" s="31"/>
+    </row>
+    <row r="69" spans="6:6">
+      <c r="F69" s="31"/>
+    </row>
+    <row r="70" spans="6:6">
+      <c r="F70" s="31"/>
+    </row>
+    <row r="71" spans="6:6">
+      <c r="F71" s="31"/>
+    </row>
+    <row r="72" spans="6:6">
+      <c r="F72" s="31"/>
+    </row>
+    <row r="73" spans="6:6">
+      <c r="F73" s="31"/>
+    </row>
+    <row r="74" spans="6:6">
+      <c r="F74" s="31"/>
+    </row>
+    <row r="75" spans="6:6">
+      <c r="F75" s="31"/>
+    </row>
+    <row r="76" spans="6:6">
+      <c r="F76" s="31"/>
+    </row>
+    <row r="77" spans="6:6">
+      <c r="F77" s="31"/>
+    </row>
+    <row r="78" spans="6:6">
+      <c r="F78" s="31"/>
+    </row>
+    <row r="79" spans="6:6">
+      <c r="F79" s="31"/>
+    </row>
+    <row r="80" spans="6:6">
+      <c r="F80" s="31"/>
+    </row>
+    <row r="81" spans="6:6">
+      <c r="F81" s="31"/>
+    </row>
+    <row r="82" spans="6:6">
+      <c r="F82" s="31"/>
+    </row>
+    <row r="83" spans="6:6">
+      <c r="F83" s="31"/>
+    </row>
+    <row r="84" spans="6:6">
+      <c r="F84" s="31"/>
+    </row>
+    <row r="85" spans="6:6">
+      <c r="F85" s="31"/>
+    </row>
+    <row r="86" spans="6:6">
+      <c r="F86" s="31"/>
+    </row>
+    <row r="87" spans="6:6">
+      <c r="F87" s="31"/>
+    </row>
+    <row r="88" spans="6:6">
+      <c r="F88" s="31"/>
+    </row>
+    <row r="89" spans="6:6">
+      <c r="F89" s="31"/>
+    </row>
+    <row r="90" spans="6:6">
+      <c r="F90" s="31"/>
+    </row>
+    <row r="91" spans="6:6">
+      <c r="F91" s="31"/>
+    </row>
+    <row r="92" spans="6:6">
+      <c r="F92" s="31"/>
+    </row>
+    <row r="93" spans="6:6">
+      <c r="F93" s="31"/>
+    </row>
+    <row r="94" spans="6:6">
+      <c r="F94" s="31"/>
+    </row>
+    <row r="95" spans="6:6">
+      <c r="F95" s="31"/>
+    </row>
+    <row r="96" spans="6:6">
+      <c r="F96" s="31"/>
+    </row>
+    <row r="97" spans="6:6">
+      <c r="F97" s="31"/>
+    </row>
+    <row r="98" spans="6:6">
+      <c r="F98" s="31"/>
+    </row>
+    <row r="99" spans="6:6">
+      <c r="F99" s="31"/>
+    </row>
+    <row r="100" spans="6:6">
+      <c r="F100" s="31"/>
+    </row>
+    <row r="101" spans="6:6">
+      <c r="F101" s="31"/>
+    </row>
+    <row r="102" spans="6:6">
+      <c r="F102" s="31"/>
+    </row>
+    <row r="103" spans="6:6">
+      <c r="F103" s="31"/>
+    </row>
+    <row r="104" spans="6:6">
+      <c r="F104" s="31"/>
+    </row>
+    <row r="105" spans="6:6">
+      <c r="F105" s="31"/>
+    </row>
+    <row r="106" spans="6:6">
+      <c r="F106" s="31"/>
+    </row>
+    <row r="107" spans="6:6">
+      <c r="F107" s="31"/>
+    </row>
+    <row r="108" spans="6:6">
+      <c r="F108" s="31"/>
+    </row>
+    <row r="109" spans="6:6">
+      <c r="F109" s="31"/>
+    </row>
+    <row r="110" spans="6:6">
+      <c r="F110" s="31"/>
+    </row>
+    <row r="111" spans="6:6">
+      <c r="F111" s="31"/>
+    </row>
+    <row r="112" spans="6:6">
+      <c r="F112" s="31"/>
+    </row>
+    <row r="113" spans="6:6">
+      <c r="F113" s="31"/>
+    </row>
+    <row r="114" spans="6:6">
+      <c r="F114" s="31"/>
+    </row>
+    <row r="115" spans="6:6">
+      <c r="F115" s="31"/>
+    </row>
+    <row r="116" spans="6:6">
+      <c r="F116" s="31"/>
+    </row>
+    <row r="117" spans="6:6">
+      <c r="F117" s="31"/>
+    </row>
+    <row r="118" spans="6:6">
+      <c r="F118" s="31"/>
+    </row>
+    <row r="119" spans="6:6">
+      <c r="F119" s="31"/>
+    </row>
+    <row r="120" spans="6:6">
+      <c r="F120" s="31"/>
+    </row>
+    <row r="121" spans="6:6">
+      <c r="F121" s="31"/>
+    </row>
+    <row r="122" spans="6:6">
+      <c r="F122" s="31"/>
+    </row>
+    <row r="123" spans="6:6">
+      <c r="F123" s="31"/>
+    </row>
+    <row r="124" spans="6:6">
+      <c r="F124" s="31"/>
+    </row>
+    <row r="125" spans="6:6">
+      <c r="F125" s="31"/>
+    </row>
+    <row r="126" spans="6:6">
+      <c r="F126" s="31"/>
+    </row>
+    <row r="127" spans="6:6">
+      <c r="F127" s="31"/>
+    </row>
+    <row r="128" spans="6:6">
+      <c r="F128" s="31"/>
+    </row>
+    <row r="129" spans="6:6">
+      <c r="F129" s="31"/>
+    </row>
+    <row r="130" spans="6:6">
+      <c r="F130" s="31"/>
+    </row>
+    <row r="131" spans="6:6">
+      <c r="F131" s="31"/>
+    </row>
+    <row r="132" spans="6:6">
+      <c r="F132" s="31"/>
+    </row>
+    <row r="133" spans="6:6">
+      <c r="F133" s="31"/>
+    </row>
+    <row r="134" spans="6:6">
+      <c r="F134" s="31"/>
+    </row>
+    <row r="135" spans="6:6">
+      <c r="F135" s="31"/>
+    </row>
+    <row r="136" spans="6:6">
+      <c r="F136" s="31"/>
+    </row>
+    <row r="137" spans="6:6">
+      <c r="F137" s="31"/>
+    </row>
+    <row r="138" spans="6:6">
+      <c r="F138" s="31"/>
+    </row>
+    <row r="139" spans="6:6">
+      <c r="F139" s="31"/>
+    </row>
+    <row r="140" spans="6:6">
+      <c r="F140" s="31"/>
+    </row>
+    <row r="141" spans="6:6">
+      <c r="F141" s="31"/>
+    </row>
+    <row r="142" spans="6:6">
+      <c r="F142" s="31"/>
+    </row>
+    <row r="143" spans="6:6">
+      <c r="F143" s="31"/>
+    </row>
+    <row r="144" spans="6:6">
+      <c r="F144" s="31"/>
+    </row>
+    <row r="145" spans="6:6">
+      <c r="F145" s="31"/>
+    </row>
+    <row r="146" spans="6:6">
+      <c r="F146" s="31"/>
+    </row>
+    <row r="147" spans="6:6">
+      <c r="F147" s="31"/>
+    </row>
+    <row r="148" spans="6:6">
+      <c r="F148" s="31"/>
+    </row>
+    <row r="149" spans="6:6">
+      <c r="F149" s="31"/>
+    </row>
+    <row r="150" spans="6:6">
+      <c r="F150" s="31"/>
+    </row>
+    <row r="151" spans="6:6">
+      <c r="F151" s="31"/>
+    </row>
+    <row r="152" spans="6:6">
+      <c r="F152" s="31"/>
+    </row>
+    <row r="153" spans="6:6">
+      <c r="F153" s="31"/>
+    </row>
+    <row r="154" spans="6:6">
+      <c r="F154" s="31"/>
+    </row>
+    <row r="155" spans="6:6">
+      <c r="F155" s="31"/>
+    </row>
+    <row r="156" spans="6:6">
+      <c r="F156" s="31"/>
+    </row>
+    <row r="157" spans="6:6">
+      <c r="F157" s="31"/>
+    </row>
+    <row r="158" spans="6:6">
+      <c r="F158" s="31"/>
+    </row>
+    <row r="159" spans="6:6">
+      <c r="F159" s="31"/>
+    </row>
+    <row r="160" spans="6:6">
+      <c r="F160" s="31"/>
+    </row>
+    <row r="161" spans="6:6">
+      <c r="F161" s="31"/>
+    </row>
+    <row r="162" spans="6:6">
+      <c r="F162" s="31"/>
+    </row>
+    <row r="163" spans="6:6">
+      <c r="F163" s="31"/>
+    </row>
+    <row r="164" spans="6:6">
+      <c r="F164" s="31"/>
+    </row>
+    <row r="165" spans="6:6">
+      <c r="F165" s="31"/>
+    </row>
+    <row r="166" spans="6:6">
+      <c r="F166" s="31"/>
+    </row>
+    <row r="167" spans="6:6">
+      <c r="F167" s="31"/>
+    </row>
+    <row r="168" spans="6:6">
+      <c r="F168" s="31"/>
+    </row>
+    <row r="169" spans="6:6">
+      <c r="F169" s="31"/>
+    </row>
+    <row r="170" spans="6:6">
+      <c r="F170" s="31"/>
+    </row>
+    <row r="171" spans="6:6">
+      <c r="F171" s="31"/>
+    </row>
+    <row r="172" spans="6:6">
+      <c r="F172" s="31"/>
+    </row>
+    <row r="173" spans="6:6">
+      <c r="F173" s="31"/>
+    </row>
+    <row r="174" spans="6:6">
+      <c r="F174" s="31"/>
+    </row>
+    <row r="175" spans="6:6">
+      <c r="F175" s="31"/>
+    </row>
+    <row r="176" spans="6:6">
+      <c r="F176" s="31"/>
+    </row>
+    <row r="177" spans="6:6">
+      <c r="F177" s="31"/>
+    </row>
+    <row r="178" spans="6:6">
+      <c r="F178" s="31"/>
+    </row>
+    <row r="179" spans="6:6">
+      <c r="F179" s="31"/>
+    </row>
+    <row r="180" spans="6:6">
+      <c r="F180" s="31"/>
+    </row>
+    <row r="181" spans="6:6">
+      <c r="F181" s="31"/>
+    </row>
+    <row r="182" spans="6:6">
+      <c r="F182" s="31"/>
+    </row>
+    <row r="183" spans="6:6">
+      <c r="F183" s="31"/>
+    </row>
+    <row r="184" spans="6:6">
+      <c r="F184" s="31"/>
+    </row>
+    <row r="185" spans="6:6">
+      <c r="F185" s="31"/>
+    </row>
+    <row r="186" spans="6:6">
+      <c r="F186" s="31"/>
+    </row>
+    <row r="187" spans="6:6">
+      <c r="F187" s="31"/>
+    </row>
+    <row r="188" spans="6:6">
+      <c r="F188" s="31"/>
+    </row>
+    <row r="189" spans="6:6">
+      <c r="F189" s="31"/>
+    </row>
+    <row r="190" spans="6:6">
+      <c r="F190" s="31"/>
+    </row>
+    <row r="191" spans="6:6">
+      <c r="F191" s="31"/>
+    </row>
+    <row r="192" spans="6:6">
+      <c r="F192" s="31"/>
+    </row>
+    <row r="193" spans="6:6">
+      <c r="F193" s="31"/>
+    </row>
+    <row r="194" spans="6:6">
+      <c r="F194" s="31"/>
+    </row>
+    <row r="195" spans="6:6">
+      <c r="F195" s="31"/>
+    </row>
+    <row r="196" spans="6:6">
+      <c r="F196" s="31"/>
+    </row>
+    <row r="197" spans="6:6">
+      <c r="F197" s="31"/>
+    </row>
+    <row r="198" spans="6:6">
+      <c r="F198" s="31"/>
+    </row>
+    <row r="199" spans="6:6">
+      <c r="F199" s="31"/>
+    </row>
+    <row r="200" spans="6:6">
+      <c r="F200" s="31"/>
+    </row>
+    <row r="201" spans="6:6">
+      <c r="F201" s="31"/>
+    </row>
+    <row r="202" spans="6:6">
+      <c r="F202" s="31"/>
+    </row>
+    <row r="203" spans="6:6">
+      <c r="F203" s="31"/>
+    </row>
+    <row r="204" spans="6:6">
+      <c r="F204" s="31"/>
+    </row>
+    <row r="205" spans="6:6">
+      <c r="F205" s="31"/>
+    </row>
+    <row r="206" spans="6:6">
+      <c r="F206" s="31"/>
+    </row>
+    <row r="207" spans="6:6">
+      <c r="F207" s="31"/>
+    </row>
+    <row r="208" spans="6:6">
+      <c r="F208" s="31"/>
+    </row>
+    <row r="209" spans="6:6">
+      <c r="F209" s="31"/>
+    </row>
+    <row r="210" spans="6:6">
+      <c r="F210" s="31"/>
+    </row>
+    <row r="211" spans="6:6">
+      <c r="F211" s="31"/>
+    </row>
+    <row r="212" spans="6:6">
+      <c r="F212" s="31"/>
+    </row>
+    <row r="213" spans="6:6">
+      <c r="F213" s="31"/>
+    </row>
+    <row r="214" spans="6:6">
+      <c r="F214" s="31"/>
+    </row>
+    <row r="215" spans="6:6">
+      <c r="F215" s="31"/>
+    </row>
+    <row r="216" spans="6:6">
+      <c r="F216" s="31"/>
+    </row>
+    <row r="217" spans="6:6">
+      <c r="F217" s="31"/>
+    </row>
+    <row r="218" spans="6:6">
+      <c r="F218" s="31"/>
+    </row>
+    <row r="219" spans="6:6">
+      <c r="F219" s="31"/>
+    </row>
+    <row r="220" spans="6:6">
+      <c r="F220" s="31"/>
+    </row>
+    <row r="221" spans="6:6">
+      <c r="F221" s="31"/>
+    </row>
+    <row r="222" spans="6:6">
+      <c r="F222" s="31"/>
+    </row>
+    <row r="223" spans="6:6">
+      <c r="F223" s="31"/>
+    </row>
+    <row r="224" spans="6:6">
+      <c r="F224" s="31"/>
+    </row>
+    <row r="225" spans="6:6">
+      <c r="F225" s="31"/>
+    </row>
+    <row r="226" spans="6:6">
+      <c r="F226" s="31"/>
+    </row>
+    <row r="227" spans="6:6">
+      <c r="F227" s="31"/>
+    </row>
+    <row r="228" spans="6:6">
+      <c r="F228" s="31"/>
+    </row>
+    <row r="229" spans="6:6">
+      <c r="F229" s="31"/>
+    </row>
+    <row r="230" spans="6:6">
+      <c r="F230" s="31"/>
+    </row>
+    <row r="231" spans="6:6">
+      <c r="F231" s="31"/>
+    </row>
+    <row r="232" spans="6:6">
+      <c r="F232" s="31"/>
+    </row>
+    <row r="233" spans="6:6">
+      <c r="F233" s="31"/>
+    </row>
+    <row r="234" spans="6:6">
+      <c r="F234" s="31"/>
+    </row>
+    <row r="235" spans="6:6">
+      <c r="F235" s="31"/>
+    </row>
+    <row r="236" spans="6:6">
+      <c r="F236" s="31"/>
+    </row>
+    <row r="237" spans="6:6">
+      <c r="F237" s="31"/>
+    </row>
+    <row r="238" spans="6:6">
+      <c r="F238" s="31"/>
+    </row>
+    <row r="239" spans="6:6">
+      <c r="F239" s="31"/>
+    </row>
+    <row r="240" spans="6:6">
+      <c r="F240" s="31"/>
+    </row>
+    <row r="241" spans="6:6">
+      <c r="F241" s="31"/>
+    </row>
+    <row r="242" spans="6:6">
+      <c r="F242" s="31"/>
+    </row>
+    <row r="243" spans="6:6">
+      <c r="F243" s="31"/>
+    </row>
+    <row r="244" spans="6:6">
+      <c r="F244" s="31"/>
+    </row>
+    <row r="245" spans="6:6">
+      <c r="F245" s="31"/>
+    </row>
+    <row r="246" spans="6:6">
+      <c r="F246" s="31"/>
+    </row>
+    <row r="247" spans="6:6">
+      <c r="F247" s="31"/>
+    </row>
+    <row r="248" spans="6:6">
+      <c r="F248" s="31"/>
+    </row>
+    <row r="249" spans="6:6">
+      <c r="F249" s="31"/>
+    </row>
+    <row r="250" spans="6:6">
+      <c r="F250" s="31"/>
+    </row>
+    <row r="251" spans="6:6">
+      <c r="F251" s="31"/>
+    </row>
+    <row r="252" spans="6:6">
+      <c r="F252" s="31"/>
+    </row>
+    <row r="253" spans="6:6">
+      <c r="F253" s="31"/>
+    </row>
+    <row r="254" spans="6:6">
+      <c r="F254" s="31"/>
+    </row>
+    <row r="255" spans="6:6">
+      <c r="F255" s="31"/>
+    </row>
+    <row r="256" spans="6:6">
+      <c r="F256" s="31"/>
+    </row>
+    <row r="257" spans="6:6">
+      <c r="F257" s="31"/>
+    </row>
+    <row r="258" spans="6:6">
+      <c r="F258" s="31"/>
+    </row>
+    <row r="259" spans="6:6">
+      <c r="F259" s="31"/>
+    </row>
+    <row r="260" spans="6:6">
+      <c r="F260" s="31"/>
+    </row>
+    <row r="261" spans="6:6">
+      <c r="F261" s="31"/>
+    </row>
+    <row r="262" spans="6:6">
+      <c r="F262" s="31"/>
+    </row>
+    <row r="263" spans="6:6">
+      <c r="F263" s="31"/>
+    </row>
+    <row r="264" spans="6:6">
+      <c r="F264" s="31"/>
+    </row>
+    <row r="265" spans="6:6">
+      <c r="F265" s="31"/>
+    </row>
+    <row r="266" spans="6:6">
+      <c r="F266" s="31"/>
+    </row>
+    <row r="267" spans="6:6">
+      <c r="F267" s="31"/>
+    </row>
+    <row r="268" spans="6:6">
+      <c r="F268" s="31"/>
+    </row>
+    <row r="269" spans="6:6">
+      <c r="F269" s="31"/>
+    </row>
+    <row r="270" spans="6:6">
+      <c r="F270" s="31"/>
+    </row>
+    <row r="271" spans="6:6">
+      <c r="F271" s="31"/>
+    </row>
+    <row r="272" spans="6:6">
+      <c r="F272" s="31"/>
+    </row>
+    <row r="273" spans="6:6">
+      <c r="F273" s="31"/>
+    </row>
+    <row r="274" spans="6:6">
+      <c r="F274" s="31"/>
+    </row>
+    <row r="275" spans="6:6">
+      <c r="F275" s="31"/>
+    </row>
+    <row r="276" spans="6:6">
+      <c r="F276" s="31"/>
+    </row>
+    <row r="277" spans="6:6">
+      <c r="F277" s="31"/>
+    </row>
+    <row r="278" spans="6:6">
+      <c r="F278" s="31"/>
+    </row>
+    <row r="279" spans="6:6">
+      <c r="F279" s="31"/>
+    </row>
+    <row r="280" spans="6:6">
+      <c r="F280" s="31"/>
+    </row>
+    <row r="281" spans="6:6">
+      <c r="F281" s="31"/>
+    </row>
+    <row r="282" spans="6:6">
+      <c r="F282" s="31"/>
+    </row>
+    <row r="283" spans="6:6">
+      <c r="F283" s="31"/>
+    </row>
+    <row r="284" spans="6:6">
+      <c r="F284" s="31"/>
+    </row>
+    <row r="285" spans="6:6">
+      <c r="F285" s="31"/>
+    </row>
+    <row r="286" spans="6:6">
+      <c r="F286" s="31"/>
+    </row>
+    <row r="287" spans="6:6">
+      <c r="F287" s="31"/>
+    </row>
+    <row r="288" spans="6:6">
+      <c r="F288" s="31"/>
+    </row>
+    <row r="289" spans="6:6">
+      <c r="F289" s="31"/>
+    </row>
+    <row r="290" spans="6:6">
+      <c r="F290" s="31"/>
+    </row>
+    <row r="291" spans="6:6">
+      <c r="F291" s="31"/>
+    </row>
+    <row r="292" spans="6:6">
+      <c r="F292" s="31"/>
+    </row>
+    <row r="293" spans="6:6">
+      <c r="F293" s="31"/>
+    </row>
+    <row r="294" spans="6:6">
+      <c r="F294" s="31"/>
+    </row>
+    <row r="295" spans="6:6">
+      <c r="F295" s="31"/>
+    </row>
+    <row r="296" spans="6:6">
+      <c r="F296" s="31"/>
+    </row>
+    <row r="297" spans="6:6">
+      <c r="F297" s="31"/>
+    </row>
+    <row r="298" spans="6:6">
+      <c r="F298" s="31"/>
+    </row>
+    <row r="299" spans="6:6">
+      <c r="F299" s="31"/>
+    </row>
+    <row r="300" spans="6:6">
+      <c r="F300" s="31"/>
+    </row>
+    <row r="301" spans="6:6">
+      <c r="F301" s="31"/>
+    </row>
+    <row r="302" spans="6:6">
+      <c r="F302" s="31"/>
+    </row>
+    <row r="303" spans="6:6">
+      <c r="F303" s="31"/>
+    </row>
+    <row r="304" spans="6:6">
+      <c r="F304" s="31"/>
+    </row>
+    <row r="305" spans="6:6">
+      <c r="F305" s="31"/>
+    </row>
+    <row r="306" spans="6:6">
+      <c r="F306" s="31"/>
+    </row>
+    <row r="307" spans="6:6">
+      <c r="F307" s="31"/>
+    </row>
+    <row r="308" spans="6:6">
+      <c r="F308" s="31"/>
+    </row>
+    <row r="309" spans="6:6">
+      <c r="F309" s="31"/>
+    </row>
+    <row r="310" spans="6:6">
+      <c r="F310" s="31"/>
+    </row>
+    <row r="311" spans="6:6">
+      <c r="F311" s="31"/>
+    </row>
+    <row r="312" spans="6:6">
+      <c r="F312" s="31"/>
+    </row>
+    <row r="313" spans="6:6">
+      <c r="F313" s="31"/>
+    </row>
+    <row r="314" spans="6:6">
+      <c r="F314" s="31"/>
+    </row>
+    <row r="315" spans="6:6">
+      <c r="F315" s="31"/>
+    </row>
+    <row r="316" spans="6:6">
+      <c r="F316" s="31"/>
+    </row>
+    <row r="317" spans="6:6">
+      <c r="F317" s="31"/>
+    </row>
+    <row r="318" spans="6:6">
+      <c r="F318" s="31"/>
+    </row>
+    <row r="319" spans="6:6">
+      <c r="F319" s="31"/>
+    </row>
+    <row r="320" spans="6:6">
+      <c r="F320" s="31"/>
+    </row>
+    <row r="321" spans="6:6">
+      <c r="F321" s="31"/>
+    </row>
+    <row r="322" spans="6:6">
+      <c r="F322" s="31"/>
+    </row>
+    <row r="323" spans="6:6">
+      <c r="F323" s="31"/>
+    </row>
+    <row r="324" spans="6:6">
+      <c r="F324" s="31"/>
+    </row>
+    <row r="325" spans="6:6">
+      <c r="F325" s="31"/>
+    </row>
+    <row r="326" spans="6:6">
+      <c r="F326" s="31"/>
+    </row>
+    <row r="327" spans="6:6">
+      <c r="F327" s="31"/>
+    </row>
+    <row r="328" spans="6:6">
+      <c r="F328" s="31"/>
+    </row>
+    <row r="329" spans="6:6">
+      <c r="F329" s="31"/>
+    </row>
+    <row r="330" spans="6:6">
+      <c r="F330" s="31"/>
+    </row>
+    <row r="331" spans="6:6">
+      <c r="F331" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3502,24 +3574,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>